<commit_message>
1.3 CSS and XPath works. 100 sec timeout removed.
</commit_message>
<xml_diff>
--- a/sample-tests.xlsx
+++ b/sample-tests.xlsx
@@ -403,7 +403,7 @@
   <dimension ref="A1:N54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="E53" activeCellId="0" sqref="E53"/>
     </sheetView>
@@ -875,7 +875,7 @@
         <v>15</v>
       </c>
       <c r="E53" s="1" t="n">
-        <v>30</v>
+        <v>300000</v>
       </c>
     </row>
     <row r="54" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
1.3.2 release ready with readme. no npm install.
</commit_message>
<xml_diff>
--- a/sample-tests.xlsx
+++ b/sample-tests.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="61">
   <si>
     <t xml:space="preserve">Desc</t>
   </si>
@@ -400,12 +400,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N54"/>
+  <dimension ref="A1:N53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E53" activeCellId="0" sqref="E53"/>
+      <selection pane="bottomLeft" activeCell="C56" activeCellId="0" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -870,16 +870,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D53" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E53" s="1" t="n">
-        <v>300000</v>
-      </c>
-    </row>
-    <row r="54" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="4" t="s">
+    <row r="53" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="4" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1.4.0 wait and wait:click works.
</commit_message>
<xml_diff>
--- a/sample-tests.xlsx
+++ b/sample-tests.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="66">
   <si>
     <t xml:space="preserve">Desc</t>
   </si>
@@ -186,6 +186,21 @@
   </si>
   <si>
     <t xml:space="preserve">div.percenttext</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Case 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JQuery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//button[@id='downloadButton'] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">//button[contains(text(),'Close')] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait:click</t>
   </si>
   <si>
     <t xml:space="preserve">End</t>
@@ -213,7 +228,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -234,6 +249,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -290,7 +310,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -323,14 +343,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -400,22 +424,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N53"/>
+  <dimension ref="A1:N59"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C56" activeCellId="0" sqref="C56"/>
+      <selection pane="bottomLeft" activeCell="C54" activeCellId="0" sqref="C54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.63"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -843,13 +866,14 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="7" t="s">
         <v>53</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>30</v>
       </c>
+      <c r="E50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D51" s="0" t="s">
@@ -873,6 +897,54 @@
     <row r="53" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C54" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C55" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C56" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C57" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C58" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E58" s="1" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="59" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="4" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -897,10 +969,7 @@
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="23.39"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="23.41796875" defaultRowHeight="13.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -932,7 +1001,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>9</v>
@@ -944,26 +1013,26 @@
         <v>10</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C5" s="7" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>21</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C6" s="7" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="E6" s="1"/>
     </row>

</xml_diff>